<commit_message>
Changed data in AppData.xlsx
</commit_message>
<xml_diff>
--- a/ApplicationTestData/AppData.xlsx
+++ b/ApplicationTestData/AppData.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">sagarulane@gmail.com</t>
+    <t xml:space="preserve">username</t>
   </si>
   <si>
-    <t xml:space="preserve">Welcome@2</t>
+    <t xml:space="preserve">password</t>
   </si>
 </sst>
 </file>
@@ -136,12 +136,13 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -153,10 +154,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="sagarulane@gmail.com"/>
-    <hyperlink ref="B1" r:id="rId2" display="Welcome@2"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>